<commit_message>
tdf#112306: containsSemiMixedTypes is true for blanks-only
Also export containsNonDate

Change-Id: I16283a272d51e6c305f8c381c359168c1e3848a8
Reviewed-on: https://gerrit.libreoffice.org/42130
Tested-by: Jenkins <ci@libreoffice.org>
Reviewed-by: Mike Kaganski <mike.kaganski@collabora.com>
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/pivot-table/with-strings-integers-and-dates.xlsx
+++ b/sc/qa/unit/data/xlsx/pivot-table/with-strings-integers-and-dates.xlsx
@@ -1,75 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kosiorek\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sources\lo-core1\sc\qa\unit\data\xlsx\pivot-table\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10656"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16305" windowHeight="9075"/>
   </bookViews>
   <sheets>
-    <sheet name="SheetWithPivot" sheetId="7" r:id="rId1"/>
-    <sheet name="SheetWithData" sheetId="1" r:id="rId2"/>
+    <sheet name="PivotTable" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171026" concurrentCalc="0"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+  <si>
+    <t>mixed strings and empty</t>
+  </si>
+  <si>
+    <t>mixed empty fields and integers</t>
+  </si>
+  <si>
+    <t>all fields are integers</t>
+  </si>
+  <si>
+    <t>mixed strings and integers</t>
+  </si>
+  <si>
+    <t>date and time with duplicated entries</t>
+  </si>
+  <si>
+    <t>maciej</t>
+  </si>
+  <si>
+    <t>bartosz</t>
+  </si>
+  <si>
+    <t>tekst</t>
+  </si>
+  <si>
+    <t>kosiorek</t>
+  </si>
+  <si>
+    <t>grzegorz</t>
+  </si>
+  <si>
+    <t>blank</t>
+  </si>
   <si>
     <t>Row Labels</t>
   </si>
   <si>
-    <t>bartosz</t>
-  </si>
-  <si>
-    <t>grzegorz</t>
-  </si>
-  <si>
-    <t>kosiorek</t>
-  </si>
-  <si>
-    <t>maciej</t>
-  </si>
-  <si>
     <t>(blank)</t>
   </si>
   <si>
     <t>Grand Total</t>
-  </si>
-  <si>
-    <t>mixed strings and empty</t>
-  </si>
-  <si>
-    <t>mixed empty fileds and integers</t>
-  </si>
-  <si>
-    <t>all fields are integers</t>
-  </si>
-  <si>
-    <t>mixed strings and integers</t>
-  </si>
-  <si>
-    <t>date and time with duplicated entries</t>
-  </si>
-  <si>
-    <t>tekst</t>
   </si>
   <si>
     <t>Sum of all fields are integers</t>
@@ -78,9 +78,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -88,6 +88,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -113,12 +114,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,11 +138,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Bartosz Kosiorek" refreshedDate="42970.77109652778" createdVersion="4" refreshedVersion="5" minRefreshableVersion="3" recordCount="5">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Mike Kaganski" refreshedDate="42988.312118055554" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="5">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A2:E7" sheet="SheetWithData"/>
+    <worksheetSource ref="A2:F7" sheet="Data"/>
   </cacheSource>
-  <cacheFields count="5">
+  <cacheFields count="6">
     <cacheField name="mixed strings and empty" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
         <s v="maciej"/>
@@ -151,12 +152,8 @@
         <s v="grzegorz"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="mixed empty fileds and integers" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="111" maxValue="222" count="3">
-        <m/>
-        <n v="111"/>
-        <n v="222"/>
-      </sharedItems>
+    <cacheField name="mixed empty fields and integers" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="111" maxValue="222"/>
     </cacheField>
     <cacheField name="all fields are integers" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1111" maxValue="5555"/>
@@ -167,6 +164,9 @@
     <cacheField name="date and time with duplicated entries" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-31T00:00:00" maxDate="2009-07-06T10:53:02"/>
     </cacheField>
+    <cacheField name="blank" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -180,65 +180,66 @@
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="5">
   <r>
     <x v="0"/>
-    <x v="0"/>
+    <m/>
     <n v="1111"/>
     <n v="2345"/>
     <d v="1899-12-31T00:00:00"/>
+    <m/>
   </r>
   <r>
     <x v="1"/>
-    <x v="1"/>
+    <n v="111"/>
     <n v="2222"/>
     <s v="tekst"/>
     <d v="1899-12-31T00:00:00"/>
+    <m/>
   </r>
   <r>
     <x v="2"/>
-    <x v="2"/>
+    <n v="222"/>
     <n v="3333"/>
     <n v="1234"/>
     <d v="1982-02-18T16:04:48"/>
+    <m/>
   </r>
   <r>
     <x v="3"/>
-    <x v="0"/>
+    <m/>
     <n v="4444"/>
     <s v="tekst"/>
     <d v="2009-07-06T10:53:02"/>
+    <m/>
   </r>
   <r>
     <x v="4"/>
-    <x v="0"/>
+    <m/>
     <n v="5555"/>
     <n v="5678"/>
     <d v="1936-03-23T04:48:00"/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="5">
+  <pivotFields count="6">
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="6">
         <item x="1"/>
         <item x="4"/>
         <item x="3"/>
         <item x="0"/>
         <item x="2"/>
+        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField numFmtId="164" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="164" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
@@ -298,7 +299,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -310,7 +311,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -327,9 +328,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -357,14 +358,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -392,6 +410,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -550,66 +585,65 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3">
-        <v>2222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3">
-        <v>5555</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3">
-        <v>4444</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3">
-        <v>3333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3">
+      <c r="B9" s="4">
         <v>16665</v>
       </c>
     </row>
@@ -620,38 +654,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E7"/>
+  <dimension ref="A2:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>1111</v>
@@ -659,13 +699,13 @@
       <c r="D3">
         <v>2345</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>111</v>
@@ -674,13 +714,13 @@
         <v>2222</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="4">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>222</v>
       </c>
@@ -690,27 +730,27 @@
       <c r="D5">
         <v>1234</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="1">
         <v>30000.67</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>4444</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="4">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
         <v>40000.453500000003</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>5555</v>
@@ -718,7 +758,7 @@
       <c r="D7">
         <v>5678</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="1">
         <v>13232.2</v>
       </c>
     </row>

</xml_diff>